<commit_message>
la til masse greier
</commit_message>
<xml_diff>
--- a/seq-diagram.xlsx
+++ b/seq-diagram.xlsx
@@ -214,14 +214,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -559,14 +559,14 @@
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="2"/>
@@ -602,7 +602,7 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -619,7 +619,7 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
@@ -631,13 +631,13 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="D10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="H10" s="8"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
@@ -652,7 +652,7 @@
       <c r="G11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>

</xml_diff>